<commit_message>
added log messages to multiple workflows
</commit_message>
<xml_diff>
--- a/P2_Performer/Results/03-28-2023/Rich Drexel - Dallas, Texas, United States of America.xlsx
+++ b/P2_Performer/Results/03-28-2023/Rich Drexel - Dallas, Texas, United States of America.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\Results\03-28-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F73116DD-EA7A-4FFE-AE11-E46F34DBEADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E889788B-0DFE-48A3-8181-2739DD98DA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3108" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{A1FAF4A7-F0BB-4497-A1BA-7F4F59656CDF}"/>
   </bookViews>
@@ -1127,14 +1127,14 @@
         <v>30</v>
       </c>
       <c r="B2" s="48">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="C2" s="11">
         <v>6</v>
       </c>
       <c r="D2" s="38">
         <f>PRODUCT(B2,C2)</f>
-        <v>870</v>
+        <v>732</v>
       </c>
       <c r="E2" s="39"/>
     </row>

</xml_diff>

<commit_message>
added flights to results template
</commit_message>
<xml_diff>
--- a/P2_Performer/Results/03-28-2023/Rich Drexel - Dallas, Texas, United States of America.xlsx
+++ b/P2_Performer/Results/03-28-2023/Rich Drexel - Dallas, Texas, United States of America.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\Results\03-28-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E889788B-0DFE-48A3-8181-2739DD98DA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{810055DF-B39C-4DEF-84EF-92E6CD703AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3108" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{A1FAF4A7-F0BB-4497-A1BA-7F4F59656CDF}"/>
   </bookViews>
@@ -134,7 +134,7 @@
     <t>Sonder at Commerce</t>
   </si>
   <si>
-    <t>Hilton Dallas/Park Cities</t>
+    <t>Locale Victory Park - Dallas</t>
   </si>
 </sst>
 </file>
@@ -1127,14 +1127,14 @@
         <v>30</v>
       </c>
       <c r="B2" s="48">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C2" s="11">
         <v>6</v>
       </c>
       <c r="D2" s="38">
         <f>PRODUCT(B2,C2)</f>
-        <v>732</v>
+        <v>672</v>
       </c>
       <c r="E2" s="39"/>
     </row>
@@ -1143,14 +1143,14 @@
         <v>31</v>
       </c>
       <c r="B3" s="49">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="C3" s="8">
         <v>6</v>
       </c>
       <c r="D3" s="38">
         <f t="shared" ref="D3:D4" si="0">PRODUCT(B3,C3)</f>
-        <v>870</v>
+        <v>672</v>
       </c>
       <c r="E3" s="39"/>
     </row>

</xml_diff>